<commit_message>
the first part of simulation outputs for larger3 water bodies (5.06 ha)
</commit_message>
<xml_diff>
--- a/SUMMARY/09-07-2014 - FP&SAV - Scheffer - shape - for shiny - larger3/simulation_summary_09-07-2014.xlsx
+++ b/SUMMARY/09-07-2014 - FP&SAV - Scheffer - shape - for shiny - larger3/simulation_summary_09-07-2014.xlsx
@@ -259,12 +259,6 @@
     <t>OUTPUT26()</t>
   </si>
   <si>
-    <t>inputTEMPLATEn.xls</t>
-  </si>
-  <si>
-    <t>~22500</t>
-  </si>
-  <si>
     <t>larger3</t>
   </si>
   <si>
@@ -281,6 +275,12 @@
   </si>
   <si>
     <t>09-07-2014 - FP&amp;SAV - Scheffer - shape - for shiny - larger3</t>
+  </si>
+  <si>
+    <t>inputTEMPLATEo.xls</t>
+  </si>
+  <si>
+    <t>~50625</t>
   </si>
 </sst>
 </file>
@@ -310,18 +310,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -401,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,7 +440,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +744,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -770,7 +763,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>17</v>
@@ -813,7 +806,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
@@ -824,7 +817,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -832,7 +825,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>52</v>
@@ -934,7 +927,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>11</v>
@@ -1144,7 +1137,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1233,8 +1226,8 @@
       <c r="E42" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="26" t="s">
-        <v>82</v>
+      <c r="F42" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1242,7 +1235,7 @@
         <v>79</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>